<commit_message>
se adiciona la clase de productos
</commit_message>
<xml_diff>
--- a/DiseñoFacturador.xlsx
+++ b/DiseñoFacturador.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="InicioSesion" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Usuario:</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Inactivar Cliente</t>
+  </si>
+  <si>
+    <t>Editar producto</t>
   </si>
 </sst>
 </file>
@@ -1072,7 +1075,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
@@ -1655,8 +1658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1692,10 +1695,12 @@
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="15"/>
+      <c r="H3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="15"/>
-      <c r="H3" s="14"/>
       <c r="I3" s="15"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>